<commit_message>
[master] laravel review fixed]
</commit_message>
<xml_diff>
--- a/review_points_mayphoowai.xlsx
+++ b/review_points_mayphoowai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,16 @@
     <sheet name="Tutorial 7" sheetId="6" r:id="rId5"/>
     <sheet name="Tutorial 8" sheetId="7" r:id="rId6"/>
     <sheet name="Tutorial 9" sheetId="8" r:id="rId7"/>
-    <sheet name="Ref." sheetId="3" r:id="rId8"/>
+    <sheet name="Tutorial 10" sheetId="9" r:id="rId8"/>
+    <sheet name="Sample Task List" sheetId="10" r:id="rId9"/>
+    <sheet name="Ref." sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="73">
   <si>
     <t>№</t>
   </si>
@@ -184,6 +186,27 @@
   </si>
   <si>
     <t>1) Pass this kind of script data from head instead of inside body</t>
+  </si>
+  <si>
+    <t>Unset session</t>
+  </si>
+  <si>
+    <t>1) you have to unset the session when logout</t>
+  </si>
+  <si>
+    <t>2 spaces</t>
+  </si>
+  <si>
+    <t>1) use indent of 2 spaces for blade.php</t>
+  </si>
+  <si>
+    <t>changed to 2spaces.</t>
+  </si>
+  <si>
+    <t>26/10/2021</t>
+  </si>
+  <si>
+    <t>MayPhooWai</t>
   </si>
   <si>
     <t>エラータイプ</t>
@@ -227,10 +250,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -254,7 +277,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,9 +290,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,13 +331,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,14 +353,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -323,23 +361,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -354,7 +406,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,42 +414,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,7 +441,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799951170384838"/>
+        <fgColor theme="5" tint="0.799920651875362"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,13 +459,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,85 +501,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,7 +537,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,7 +561,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,31 +609,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,56 +773,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -818,11 +803,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -835,20 +850,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -858,130 +893,130 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3640,6 +3675,198 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -4254,7 +4481,7 @@
   <sheetPr/>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="D3" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -5097,7 +5324,7 @@
   <sheetPr/>
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="E2" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="E2" workbookViewId="0">
       <selection activeCell="P3" sqref="P3:U3"/>
     </sheetView>
   </sheetViews>
@@ -5329,189 +5556,301 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:J22"/>
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="3" customWidth="1"/>
+    <col min="6" max="14" width="9" style="3"/>
+    <col min="15" max="15" width="13" style="3" customWidth="1"/>
+    <col min="16" max="21" width="9" style="3"/>
+    <col min="22" max="22" width="14.625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="3" customWidth="1"/>
+    <col min="24" max="24" width="32.5" style="3" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="33" customHeight="1" spans="1:24">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="24" customHeight="1" spans="1:24">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>44493</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>Ref.!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
+      <formula1>Ref.!$D$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>Ref.!$B$2:$B$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>Ref.!$C$2:$C$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
+      <formula1>Ref.!$E$2:$E$7</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="3" customWidth="1"/>
+    <col min="6" max="14" width="9" style="3"/>
+    <col min="15" max="15" width="13" style="3" customWidth="1"/>
+    <col min="16" max="21" width="9" style="3"/>
+    <col min="22" max="22" width="14.625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="3" customWidth="1"/>
+    <col min="24" max="24" width="32.5" style="3" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="33" customHeight="1" spans="1:24">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="X1" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="24" customHeight="1" spans="1:24">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>44495</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="W2" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="X2" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>Ref.!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
+      <formula1>Ref.!$D$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>Ref.!$B$2:$B$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>Ref.!$C$2:$C$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
+      <formula1>Ref.!$E$2:$E$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>